<commit_message>
Toevoegen klasse Leerling Aanpassen testen Aanpassen persistence Aanpassen PopulateDB Klas heeft lijst van leerlingen met voor- en achternaam
</commit_message>
<xml_diff>
--- a/src/data/KlasSheet.xlsx
+++ b/src/data/KlasSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devri\Documents\School\Toegepaste Informatica\2017-2018\Semester 2\Projecten\JAVA\java-g16\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DF9452-BD1B-4A73-9878-5DE483FF7419}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A92339-8C2F-455C-B253-93D90276565B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{37A04B54-B64B-4E1B-8CE5-74A5D2C70765}"/>
   </bookViews>
@@ -27,30 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Piet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nelis </t>
-  </si>
-  <si>
-    <t>Corneel</t>
-  </si>
-  <si>
-    <t>Joris</t>
-  </si>
-  <si>
-    <t>Welsey</t>
-  </si>
-  <si>
-    <t>Diaby</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
     <t>3A1</t>
   </si>
   <si>
@@ -58,6 +34,30 @@
   </si>
   <si>
     <t>3B1</t>
+  </si>
+  <si>
+    <t>Jan, Protput</t>
+  </si>
+  <si>
+    <t>Piet, De Hans</t>
+  </si>
+  <si>
+    <t>Nelis, Cornelis</t>
+  </si>
+  <si>
+    <t>Corneel, Teeuwen</t>
+  </si>
+  <si>
+    <t>Joris, Boris</t>
+  </si>
+  <si>
+    <t>Welsey, De Kleine</t>
+  </si>
+  <si>
+    <t>Diaby, Abdoulay</t>
+  </si>
+  <si>
+    <t>Thomas, Vermeel</t>
   </si>
 </sst>
 </file>
@@ -412,51 +412,52 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>